<commit_message>
add susp yellow purple cube
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="264">
   <si>
     <t>kr</t>
   </si>
@@ -647,6 +647,192 @@
   </si>
   <si>
     <t>몬스터 처치 시 15% 확률로 95의 MP  회복</t>
+  </si>
+  <si>
+    <t>공격 시 3% 확률로 오토스틸</t>
+  </si>
+  <si>
+    <t>3% Auto Steal</t>
+  </si>
+  <si>
+    <t>공격 시 1% 확률로 오토스틸</t>
+  </si>
+  <si>
+    <t>공격 시 2% 확률로 오토스틸</t>
+  </si>
+  <si>
+    <t>공격 시 5% 확률로 오토스틸</t>
+  </si>
+  <si>
+    <t>공격 시 7% 확률로 오토스틸</t>
+  </si>
+  <si>
+    <t>1% Auto Steal</t>
+  </si>
+  <si>
+    <t>2% Auto Steal</t>
+  </si>
+  <si>
+    <t>5% Auto Steal</t>
+  </si>
+  <si>
+    <t>7% Auto Steal</t>
+  </si>
+  <si>
+    <t>공격 시 3% 확률로 32의 HP 회복</t>
+  </si>
+  <si>
+    <t>공격 시 3% 확률로 32의 MP 회복</t>
+  </si>
+  <si>
+    <t>공격 시 10% 확률로 6레벨 중독효과 적용</t>
+  </si>
+  <si>
+    <t>공격 시 5% 확률로 2레벨 기절효과 적용</t>
+  </si>
+  <si>
+    <t>공격 시 10% 확률로 2레벨 슬로우효과 적용</t>
+  </si>
+  <si>
+    <t>공격 시 10% 확률로 3레벨 암흑효과 적용</t>
+  </si>
+  <si>
+    <t>공격 시 5% 확률로 2레벨 빙결효과 적용</t>
+  </si>
+  <si>
+    <t>공격 시 5% 확률로 2레벨 봉인효과 적용</t>
+  </si>
+  <si>
+    <t>3% chance to recover 32 HP on attack</t>
+  </si>
+  <si>
+    <t>3% chance to recover 32 MP on attack</t>
+  </si>
+  <si>
+    <t>10% chance to apply Lv 6 Poison on attack</t>
+  </si>
+  <si>
+    <t>5% chance to apply Lv 2 Stun on attack</t>
+  </si>
+  <si>
+    <t>10% chance to apply Lv 2 Slow on attack</t>
+  </si>
+  <si>
+    <t>10% chance to apply Lv 3 Darkness on attack</t>
+  </si>
+  <si>
+    <t>5% chance to apply Lv 2 Freeze on attack</t>
+  </si>
+  <si>
+    <t>5% chance to apply Lv 2 Seal on attack</t>
+  </si>
+  <si>
+    <t>공격 시 3% 확률로 28의 HP 회복</t>
+  </si>
+  <si>
+    <t>공격 시 3% 확률로 28의 MP 회복</t>
+  </si>
+  <si>
+    <t>공격 시 10% 확률로 5레벨 중독효과 적용</t>
+  </si>
+  <si>
+    <t>공격 시 10% 확률로 2레벨 암흑효과 적용</t>
+  </si>
+  <si>
+    <t>3% chance to recover 28 HP on attack</t>
+  </si>
+  <si>
+    <t>3% chance to recover 28 MP on attack</t>
+  </si>
+  <si>
+    <t>10% chance to apply Lv 5 Poison on attack</t>
+  </si>
+  <si>
+    <t>10% chance to apply Lv 2 Darkness on attack</t>
+  </si>
+  <si>
+    <t>피격 시 20% 확률로 21의 데미지 무시</t>
+  </si>
+  <si>
+    <t>피격 시 20% 확률로 32의 데미지 무시</t>
+  </si>
+  <si>
+    <t>피격 시 30% 확률로 43의 데미지 무시</t>
+  </si>
+  <si>
+    <t>20% chance to ignore 21 damage when attacked</t>
+  </si>
+  <si>
+    <t>20% chance to ignore 32 damage when attacked</t>
+  </si>
+  <si>
+    <t>30% chance to ignore 43 damage when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 20% 확률로 25의 데미지 무시</t>
+  </si>
+  <si>
+    <t>피격 시 20% 확률로 38의 데미지 무시</t>
+  </si>
+  <si>
+    <t>20% chance to ignore 25 damage when attacked</t>
+  </si>
+  <si>
+    <t>20% chance to ignore 38 damage when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 30% 확률로 51의 데미지 무시</t>
+  </si>
+  <si>
+    <t>30% chance to ignore 51 damage when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 10% 확률로 10초간 분노를 느낀다.</t>
+  </si>
+  <si>
+    <t>10% chance to become Angry for 10 sec when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 10% 확률로 10초간 행복을 느낀다.</t>
+  </si>
+  <si>
+    <t>10% chance to become Happy for 10 sec when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 10% 확률로 10초간 사랑에 빠진다.</t>
+  </si>
+  <si>
+    <t>10% chance to become In Love for 10 sec when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 10% 확률로 10초간 격노를 느낀다.</t>
+  </si>
+  <si>
+    <t>10% chance to become Enraged for 10 sec when attacked</t>
+  </si>
+  <si>
+    <t>피격 시 10% 확률로 10초간 감동을 느낀다.</t>
+  </si>
+  <si>
+    <t>10% chance to become Touched for 10 sec when attacked</t>
+  </si>
+  <si>
+    <t>4초 당 24의 HP 회복</t>
+  </si>
+  <si>
+    <t>Recover 24 HP every 4 seconds</t>
+  </si>
+  <si>
+    <t>4초 당 24의 MP 회복</t>
+  </si>
+  <si>
+    <t>Recover 24 MP every 4 seconds</t>
+  </si>
+  <si>
+    <t>모든 스킬레벨</t>
+  </si>
+  <si>
+    <t>모든 스킬의 재사용 대기시간</t>
   </si>
 </sst>
 </file>
@@ -969,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B102"/>
+  <dimension ref="A1:B138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,6 +1984,294 @@
         <v>198</v>
       </c>
     </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>205</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>202</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>206</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>207</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>212</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>213</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>214</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>215</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>216</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>218</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>228</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>229</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>230</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>215</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>216</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>231</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>218</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>219</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>236</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>237</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>238</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>242</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>243</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>246</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>248</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>250</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>252</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>254</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>256</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>258</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>260</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>262</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>263</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add normal pot translation
</commit_message>
<xml_diff>
--- a/translations.xlsx
+++ b/translations.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="translations_1" localSheetId="0">Book1!$A$1:$B$102</definedName>
+    <definedName name="translations_1" localSheetId="0">Book1!$A$1:$B$103</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="65001"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="266">
   <si>
     <t>kr</t>
   </si>
@@ -833,6 +833,12 @@
   </si>
   <si>
     <t>모든 스킬의 재사용 대기시간</t>
+  </si>
+  <si>
+    <t>노멀</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="F151" sqref="F151"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,937 +1344,945 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>264</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>123</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>200</v>
+        <v>84</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>86</v>
+        <v>201</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>181</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B103" s="1" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>204</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>165</v>
+        <v>261</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>262</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>263</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B139" s="1" t="s">
         <v>199</v>
       </c>
     </row>

</xml_diff>